<commit_message>
Backup QR Scanner data - 2025-10-30T23:29:01.120Z - Cache Bust: 1761866941120
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Chest_checklist1761866300877_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_Chest_checklist1761866300877_backup@backdoor.com.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Checklist" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -436,7 +436,7 @@
         <v>01:18:38</v>
       </c>
       <c r="E2" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F2" t="str">
         <v>backup@backdoor.com</v>
@@ -456,7 +456,7 @@
         <v>01:18:45</v>
       </c>
       <c r="E3" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F3" t="str">
         <v>backup@backdoor.com</v>
@@ -476,7 +476,7 @@
         <v>01:18:49</v>
       </c>
       <c r="E4" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F4" t="str">
         <v>backup@backdoor.com</v>
@@ -496,7 +496,7 @@
         <v>01:18:57</v>
       </c>
       <c r="E5" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F5" t="str">
         <v>backup@backdoor.com</v>
@@ -516,7 +516,7 @@
         <v>01:19:00</v>
       </c>
       <c r="E6" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F6" t="str">
         <v>backup@backdoor.com</v>
@@ -536,7 +536,7 @@
         <v>01:19:06</v>
       </c>
       <c r="E7" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F7" t="str">
         <v>backup@backdoor.com</v>
@@ -556,7 +556,7 @@
         <v>01:19:11</v>
       </c>
       <c r="E8" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F8" t="str">
         <v>backup@backdoor.com</v>
@@ -576,7 +576,7 @@
         <v>01:19:14</v>
       </c>
       <c r="E9" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F9" t="str">
         <v>backup@backdoor.com</v>
@@ -596,7 +596,7 @@
         <v>01:19:22</v>
       </c>
       <c r="E10" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F10" t="str">
         <v>backup@backdoor.com</v>
@@ -616,7 +616,7 @@
         <v>01:19:25</v>
       </c>
       <c r="E11" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F11" t="str">
         <v>backup@backdoor.com</v>
@@ -636,7 +636,7 @@
         <v>01:19:33</v>
       </c>
       <c r="E12" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F12" t="str">
         <v>backup@backdoor.com</v>
@@ -656,7 +656,7 @@
         <v>01:19:37</v>
       </c>
       <c r="E13" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F13" t="str">
         <v>backup@backdoor.com</v>
@@ -676,7 +676,7 @@
         <v>01:19:42</v>
       </c>
       <c r="E14" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F14" t="str">
         <v>backup@backdoor.com</v>
@@ -696,7 +696,7 @@
         <v>01:19:47</v>
       </c>
       <c r="E15" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F15" t="str">
         <v>backup@backdoor.com</v>
@@ -716,7 +716,7 @@
         <v>01:20:25</v>
       </c>
       <c r="E16" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F16" t="str">
         <v>backup@backdoor.com</v>
@@ -736,7 +736,7 @@
         <v>01:20:33</v>
       </c>
       <c r="E17" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F17" t="str">
         <v>backup@backdoor.com</v>
@@ -756,7 +756,7 @@
         <v>01:20:36</v>
       </c>
       <c r="E18" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F18" t="str">
         <v>backup@backdoor.com</v>
@@ -776,7 +776,7 @@
         <v>01:20:44</v>
       </c>
       <c r="E19" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F19" t="str">
         <v>backup@backdoor.com</v>
@@ -796,7 +796,7 @@
         <v>01:20:48</v>
       </c>
       <c r="E20" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F20" t="str">
         <v>backup@backdoor.com</v>
@@ -816,7 +816,7 @@
         <v>01:20:52</v>
       </c>
       <c r="E21" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F21" t="str">
         <v>backup@backdoor.com</v>
@@ -836,7 +836,7 @@
         <v>01:20:58</v>
       </c>
       <c r="E22" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F22" t="str">
         <v>backup@backdoor.com</v>
@@ -856,7 +856,7 @@
         <v>01:21:01</v>
       </c>
       <c r="E23" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F23" t="str">
         <v>backup@backdoor.com</v>
@@ -876,7 +876,7 @@
         <v>01:21:06</v>
       </c>
       <c r="E24" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F24" t="str">
         <v>backup@backdoor.com</v>
@@ -896,7 +896,7 @@
         <v>01:21:09</v>
       </c>
       <c r="E25" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F25" t="str">
         <v>backup@backdoor.com</v>
@@ -916,7 +916,7 @@
         <v>01:21:12</v>
       </c>
       <c r="E26" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F26" t="str">
         <v>backup@backdoor.com</v>
@@ -936,7 +936,7 @@
         <v>01:21:20</v>
       </c>
       <c r="E27" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F27" t="str">
         <v>backup@backdoor.com</v>
@@ -956,7 +956,7 @@
         <v>01:21:22</v>
       </c>
       <c r="E28" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F28" t="str">
         <v>backup@backdoor.com</v>
@@ -976,7 +976,7 @@
         <v>01:21:25</v>
       </c>
       <c r="E29" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F29" t="str">
         <v>backup@backdoor.com</v>
@@ -996,7 +996,7 @@
         <v>01:21:30</v>
       </c>
       <c r="E30" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F30" t="str">
         <v>backup@backdoor.com</v>
@@ -1016,7 +1016,7 @@
         <v>01:22:30</v>
       </c>
       <c r="E31" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F31" t="str">
         <v>backup@backdoor.com</v>
@@ -1036,7 +1036,7 @@
         <v>01:22:33</v>
       </c>
       <c r="E32" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F32" t="str">
         <v>backup@backdoor.com</v>
@@ -1056,7 +1056,7 @@
         <v>01:25:12</v>
       </c>
       <c r="E33" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F33" t="str">
         <v>backup@backdoor.com</v>
@@ -1076,7 +1076,7 @@
         <v>01:25:16</v>
       </c>
       <c r="E34" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F34" t="str">
         <v>backup@backdoor.com</v>
@@ -1096,7 +1096,7 @@
         <v>01:25:21</v>
       </c>
       <c r="E35" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F35" t="str">
         <v>backup@backdoor.com</v>
@@ -1116,7 +1116,7 @@
         <v>01:25:24</v>
       </c>
       <c r="E36" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F36" t="str">
         <v>backup@backdoor.com</v>
@@ -1136,7 +1136,7 @@
         <v>01:25:28</v>
       </c>
       <c r="E37" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F37" t="str">
         <v>backup@backdoor.com</v>
@@ -1156,7 +1156,7 @@
         <v>01:25:34</v>
       </c>
       <c r="E38" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F38" t="str">
         <v>backup@backdoor.com</v>
@@ -1176,7 +1176,7 @@
         <v>01:25:39</v>
       </c>
       <c r="E39" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F39" t="str">
         <v>backup@backdoor.com</v>
@@ -1196,7 +1196,7 @@
         <v>01:25:44</v>
       </c>
       <c r="E40" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F40" t="str">
         <v>backup@backdoor.com</v>
@@ -1216,7 +1216,7 @@
         <v>01:25:57</v>
       </c>
       <c r="E41" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F41" t="str">
         <v>backup@backdoor.com</v>
@@ -1236,7 +1236,7 @@
         <v>01:26:02</v>
       </c>
       <c r="E42" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F42" t="str">
         <v>backup@backdoor.com</v>
@@ -1256,7 +1256,7 @@
         <v>01:26:06</v>
       </c>
       <c r="E43" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F43" t="str">
         <v>backup@backdoor.com</v>
@@ -1276,7 +1276,7 @@
         <v>01:26:11</v>
       </c>
       <c r="E44" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F44" t="str">
         <v>backup@backdoor.com</v>
@@ -1296,7 +1296,7 @@
         <v>01:26:15</v>
       </c>
       <c r="E45" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F45" t="str">
         <v>backup@backdoor.com</v>
@@ -1316,7 +1316,7 @@
         <v>01:26:20</v>
       </c>
       <c r="E46" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F46" t="str">
         <v>backup@backdoor.com</v>
@@ -1336,7 +1336,7 @@
         <v>01:26:27</v>
       </c>
       <c r="E47" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F47" t="str">
         <v>backup@backdoor.com</v>
@@ -1356,7 +1356,7 @@
         <v>01:26:35</v>
       </c>
       <c r="E48" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F48" t="str">
         <v>backup@backdoor.com</v>
@@ -1376,7 +1376,7 @@
         <v>01:26:39</v>
       </c>
       <c r="E49" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F49" t="str">
         <v>backup@backdoor.com</v>
@@ -1396,7 +1396,7 @@
         <v>01:26:43</v>
       </c>
       <c r="E50" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F50" t="str">
         <v>backup@backdoor.com</v>
@@ -1416,7 +1416,7 @@
         <v>01:26:47</v>
       </c>
       <c r="E51" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F51" t="str">
         <v>backup@backdoor.com</v>
@@ -1436,7 +1436,7 @@
         <v>01:27:12</v>
       </c>
       <c r="E52" t="str">
-        <v>Selection</v>
+        <v>Scan</v>
       </c>
       <c r="F52" t="str">
         <v>backup@backdoor.com</v>

</xml_diff>